<commit_message>
Update design of view. -Add area to display pressure and description.
</commit_message>
<xml_diff>
--- a/dev/doc/design/display_layout.xlsx
+++ b/dev/doc/design/display_layout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\development\QtHermometer\dev\doc\design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\development\RaspiEnvMeter\dev\doc\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>○</t>
     <phoneticPr fontId="1"/>
@@ -143,31 +143,47 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>This is trial item, because to read the value from a sensor, it is needed to access</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>analogu way but the device RaspberryPi3 does not have analog input/output pin.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>To realize the access, arduino is needed, and used to communicate via SPI communication.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>But arduino can act only as MASTER, and RaspberryPi is too.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>So, to set to make arduino or RaspberryPi3 act as SLAVE. I does not know the way.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Area marked by "E" shows the LUX.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>E)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>D)</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Area marked by "D" shows the LUX.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>This is trial item, because to read the value from a sensor, it is needed to access</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>analogu way but the device RaspberryPi3 does not have analog input/output pin.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>To realize the access, arduino is needed, and used to communicate via SPI communication.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>But arduino can act only as MASTER, and RaspberryPi is too.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>So, to set to make arduino or RaspberryPi3 act as SLAVE. I does not know the way.</t>
+    <t>Area marked by "D" shows pressure.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The unit of pressure is hPa.</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -452,7 +468,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -464,8 +480,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1066800" y="2895600"/>
-          <a:ext cx="2133600" cy="914400"/>
+          <a:off x="1219200" y="2895600"/>
+          <a:ext cx="1524000" cy="914400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -509,13 +525,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -527,7 +543,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3352800" y="2895600"/>
+          <a:off x="2895600" y="2895600"/>
           <a:ext cx="914400" cy="914400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -572,7 +588,7 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>30</xdr:col>
+      <xdr:col>31</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -590,8 +606,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4419600" y="2895600"/>
-          <a:ext cx="762000" cy="914400"/>
+          <a:off x="4724400" y="2895600"/>
+          <a:ext cx="609600" cy="914400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -684,13 +700,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>92091</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>136510</xdr:rowOff>
@@ -702,7 +718,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3276600" y="2835291"/>
+          <a:off x="2819400" y="2835291"/>
           <a:ext cx="0" cy="1111219"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -735,13 +751,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>29</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>107981</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -753,7 +769,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4343400" y="2851181"/>
+          <a:off x="4648200" y="2851181"/>
           <a:ext cx="0" cy="1111219"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1127,7 +1143,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1139,8 +1155,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1219200" y="3048000"/>
-          <a:ext cx="762000" cy="609600"/>
+          <a:off x="1371600" y="3048000"/>
+          <a:ext cx="457200" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1177,7 +1193,7 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2800" baseline="0"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0"/>
             <a:t>mm</a:t>
           </a:r>
         </a:p>
@@ -1187,13 +1203,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1205,8 +1221,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2286000" y="3048000"/>
-          <a:ext cx="762000" cy="609600"/>
+          <a:off x="2133600" y="3048000"/>
+          <a:ext cx="457200" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1243,7 +1259,7 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2800" baseline="0"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0"/>
             <a:t>dd</a:t>
           </a:r>
         </a:p>
@@ -1253,13 +1269,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1271,7 +1287,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1981200" y="3048000"/>
+          <a:off x="1828800" y="3048000"/>
           <a:ext cx="304800" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1319,13 +1335,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1337,7 +1353,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3505200" y="3048000"/>
+          <a:off x="3048000" y="3048000"/>
           <a:ext cx="457200" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1392,13 +1408,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1410,7 +1426,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3962400" y="3200400"/>
+          <a:off x="3505200" y="3200400"/>
           <a:ext cx="152400" cy="457200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1458,7 +1474,7 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>31</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1476,8 +1492,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4572000" y="3048000"/>
-          <a:ext cx="457200" cy="609600"/>
+          <a:off x="4876800" y="3048000"/>
+          <a:ext cx="304800" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1670,7 +1686,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
@@ -1683,7 +1699,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3505200" y="2895601"/>
+          <a:off x="2895600" y="2895601"/>
           <a:ext cx="304800" cy="304799"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1743,7 +1759,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>30</xdr:col>
+      <xdr:col>31</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
@@ -1756,7 +1772,267 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4572000" y="2895601"/>
+          <a:off x="4724400" y="2895601"/>
+          <a:ext cx="304800" cy="304799"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2000">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>E</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2000">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>107981</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="直線コネクタ 26"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3905250" y="2851181"/>
+          <a:ext cx="0" cy="1111219"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="正方形/長方形 31"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3962400" y="2895600"/>
+          <a:ext cx="609600" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="lgDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="テキスト ボックス 32"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4114800" y="3048000"/>
+          <a:ext cx="304800" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:srgbClr val="0000FF"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="700" baseline="0"/>
+            <a:t>Deci</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="700" baseline="0"/>
+            <a:t>mal</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304799"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="テキスト ボックス 33"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3962400" y="2895600"/>
           <a:ext cx="304800" cy="304799"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -2080,7 +2356,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H52"/>
+  <dimension ref="B2:H55"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2214,44 +2490,63 @@
         <v>21</v>
       </c>
     </row>
+    <row r="46" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="G46" s="2"/>
+    </row>
     <row r="47" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F47" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48" spans="6:8" x14ac:dyDescent="0.2">
-      <c r="G48" s="3" t="s">
+      <c r="G48" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H48" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F50" t="s">
+        <v>28</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="G51" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H51" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="G52" s="3"/>
+      <c r="H52" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="G53" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H53" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G49" s="3"/>
-      <c r="H49" t="s">
+    <row r="54" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="H54" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G50" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H50" t="s">
+    <row r="55" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="H55" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="51" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="H51" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="52" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="H52" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>